<commit_message>
update der def. Bestelllisten inkl. Budget
</commit_message>
<xml_diff>
--- a/01_Organisation/05_Bestellungen/Bestellformular_SysProjekt_18_Team10_Mechanik.xlsx
+++ b/01_Organisation/05_Bestellungen/Bestellformular_SysProjekt_18_Team10_Mechanik.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donkey Kong\Documents\GitHub\SysP18_1cv\01_Organisation\05_Bestellungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A021AD9-1A9F-4621-91B1-553FCBB1C0C3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAFA92B-77EE-4A53-9064-9344B09881A7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bestellformular_SysProjekt" sheetId="1" r:id="rId1"/>
+    <sheet name="Team 10 Mechanik" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Lieferant</t>
   </si>
@@ -82,6 +82,30 @@
   </si>
   <si>
     <t>148-21-717</t>
+  </si>
+  <si>
+    <t>182-49-575</t>
+  </si>
+  <si>
+    <t>Lötpaste</t>
+  </si>
+  <si>
+    <t>182-49-574</t>
+  </si>
+  <si>
+    <t>Dosiernadel</t>
+  </si>
+  <si>
+    <t>300-72-943</t>
+  </si>
+  <si>
+    <t>Schlitten für lineare Führungsschienen 9 mm, Vorgeschmiert ja, MNN 9-G3-LS, Schneeberger</t>
+  </si>
+  <si>
+    <t>300-72-923</t>
+  </si>
+  <si>
+    <t>Lineare Führungsschiene 9/275 mm, MN 9-275-G3-V0, Schneeberger</t>
   </si>
 </sst>
 </file>
@@ -93,7 +117,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;SFr.&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,44 +146,12 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF555555"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -240,9 +232,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -251,26 +243,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -281,12 +255,13 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -632,19 +607,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.88671875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="57.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -652,38 +627,38 @@
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18">
+      <c r="B1" s="13">
         <v>10</v>
       </c>
-      <c r="C1" s="18"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="15">
         <f ca="1">TODAY()</f>
-        <v>43195</v>
-      </c>
-      <c r="C4" s="20"/>
+        <v>43196</v>
+      </c>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -696,369 +671,368 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="12">
         <v>9.9499999999999993</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="12">
         <f t="shared" ref="F7:F30" si="0">B7*E7</f>
         <v>9.9499999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="10">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="5">
         <v>3.15</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="12">
         <f t="shared" si="0"/>
         <v>3.15</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="10">
         <v>1</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="12">
         <v>37.26</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="12">
         <f t="shared" si="0"/>
         <v>37.26</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="15">
+      <c r="A10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="12">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="F10" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="15">
+      <c r="A11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1.08</v>
+      </c>
+      <c r="F11" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="15">
+      <c r="A12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="12">
+        <v>29.67</v>
+      </c>
+      <c r="F12" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29.67</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="15">
+      <c r="A13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="10">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="12">
+        <v>45.05</v>
+      </c>
+      <c r="F13" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>45.05</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="5"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="5"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="5"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="5"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E20" s="5"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E21" s="5"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="5"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="5"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="5"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="5"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="5"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E27" s="5"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="5"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E29" s="5"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E30" s="5"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E31" s="5"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="15"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="9"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="15"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="15"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="15"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="15"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="15"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="15"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E39" s="9"/>
-      <c r="F39" s="15"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E40" s="9"/>
-      <c r="F40" s="15"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F41" s="15"/>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F42" s="15"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F43" s="15"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F44" s="15"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F45" s="15"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F46" s="15"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F47" s="15"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F48" s="15"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F49" s="15"/>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F50" s="15"/>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F51" s="15"/>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F52" s="15"/>
+      <c r="F52" s="9"/>
     </row>
     <row r="53" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F53" s="15"/>
+      <c r="F53" s="9"/>
     </row>
     <row r="54" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F54" s="15"/>
+      <c r="F54" s="9"/>
     </row>
     <row r="55" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F55" s="15"/>
+      <c r="F55" s="9"/>
     </row>
     <row r="56" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F56" s="15"/>
+      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F57" s="15"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F58" s="15"/>
+      <c r="F58" s="9"/>
     </row>
     <row r="59" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F59" s="15"/>
+      <c r="F59" s="9"/>
     </row>
     <row r="60" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F60" s="15"/>
+      <c r="F60" s="9"/>
     </row>
     <row r="61" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F61" s="15"/>
+      <c r="F61" s="9"/>
     </row>
     <row r="62" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F62" s="15"/>
+      <c r="F62" s="9"/>
     </row>
     <row r="63" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F63" s="15"/>
+      <c r="F63" s="9"/>
     </row>
     <row r="64" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F64" s="15"/>
+      <c r="F64" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>